<commit_message>
Actualizacion de los requisitos y historias de usuario en el modulo leave
</commit_message>
<xml_diff>
--- a/01-Requisitos-Historias_Usuario/Requisitos-Historias_Usuario.xlsx
+++ b/01-Requisitos-Historias_Usuario/Requisitos-Historias_Usuario.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DIEGO\Desktop\Practicas-Personales\QA\Portafolio QA Automatizacion\Requisitos-Historias_Usuario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DIEGO\Desktop\Practicas-Personales\QA\Portafolio QA Automatizacion\01-Requisitos-Historias_Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9DA58E-BDA7-4369-886C-A5D4ED884605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456FD1ED-8D6D-46EB-BD1B-DAF7003F4161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REQUISITOS" sheetId="1" r:id="rId1"/>
     <sheet name="Historias Usuario" sheetId="2" r:id="rId2"/>
+    <sheet name="HU (Module Leave)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="158">
   <si>
     <t>Requisitos Funcionales – OrangeHRM Demo</t>
   </si>
@@ -115,18 +116,6 @@
     <t>RF014</t>
   </si>
   <si>
-    <t>El sistema debe permitir a un empleado solicitar un permiso especificando tipo, fecha y motivo.</t>
-  </si>
-  <si>
-    <t>El sistema debe permitir al administrador aprobar o rechazar las solicitudes de permiso.</t>
-  </si>
-  <si>
-    <t>El sistema debe permitir al usuario visualizar el estado de sus solicitudes de permiso.</t>
-  </si>
-  <si>
-    <t>El sistema debe mostrar un calendario de permisos tomados y pendientes.</t>
-  </si>
-  <si>
     <t>Módulo Time (Asistencia)</t>
   </si>
   <si>
@@ -241,9 +230,6 @@
     <t>El sistema debe permitir exportar los reportes generados a formatos como PDF o Excel.</t>
   </si>
   <si>
-    <t>Historia de Usuario 1: Inicio de sesión</t>
-  </si>
-  <si>
     <r>
       <t>Requisito relacionado:</t>
     </r>
@@ -304,9 +290,6 @@
     <t>El botón “Login” permanece inactivo si los campos están vacíos.</t>
   </si>
   <si>
-    <t>Historia de Usuario 2: Cerrar sesión</t>
-  </si>
-  <si>
     <t>Como usuario autenticado,</t>
   </si>
   <si>
@@ -349,9 +332,6 @@
     <t>El sistema no debe permitir volver atrás con el navegador.</t>
   </si>
   <si>
-    <t>Historia de Usuario 3: Registrar nuevo empleado</t>
-  </si>
-  <si>
     <t>Como administrador,</t>
   </si>
   <si>
@@ -394,9 +374,6 @@
     <t>El empleado debe aparecer en el listado del módulo PIM.</t>
   </si>
   <si>
-    <t>Historia de Usuario 4: Editar información de empleado</t>
-  </si>
-  <si>
     <r>
       <t>quiero</t>
     </r>
@@ -436,9 +413,6 @@
     <t>Los cambios deben reflejarse en el listado.</t>
   </si>
   <si>
-    <t>Historia de Usuario 5: Buscar empleados</t>
-  </si>
-  <si>
     <r>
       <t>quiero</t>
     </r>
@@ -475,135 +449,6 @@
     <t>Si no se encuentra nada, debe aparecer “No Records Found”.</t>
   </si>
   <si>
-    <t>Historia de Usuario 6: Solicitar vacaciones</t>
-  </si>
-  <si>
-    <t>Como empleado,</t>
-  </si>
-  <si>
-    <r>
-      <t>quiero</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> registrar una solicitud de vacaciones,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>para</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> que mi supervisor la revise.</t>
-    </r>
-  </si>
-  <si>
-    <t>Selección de fechas, tipo de licencia y comentarios.</t>
-  </si>
-  <si>
-    <t>No se permite seleccionar fechas pasadas.</t>
-  </si>
-  <si>
-    <t>Al enviar la solicitud, debe quedar en estado "Pending Approval".</t>
-  </si>
-  <si>
-    <t>Historia de Usuario 7: Aprobar vacaciones</t>
-  </si>
-  <si>
-    <t>Como supervisor,</t>
-  </si>
-  <si>
-    <r>
-      <t>quiero</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> aprobar o rechazar solicitudes de vacaciones,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>para</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> gestionar la disponibilidad del personal.</t>
-    </r>
-  </si>
-  <si>
-    <t>La lista de solicitudes debe mostrarse en una bandeja de entrada.</t>
-  </si>
-  <si>
-    <t>El supervisor puede seleccionar una y aprobarla o rechazarla.</t>
-  </si>
-  <si>
-    <t>El solicitante debe recibir la notificación correspondiente.</t>
-  </si>
-  <si>
-    <t>Historia de Usuario 8: Ver historial de vacaciones</t>
-  </si>
-  <si>
-    <r>
-      <t>quiero</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ver el historial de mis solicitudes de vacaciones,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>para</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> hacer seguimiento a mis días utilizados y pendientes.</t>
-    </r>
-  </si>
-  <si>
-    <t>El historial debe incluir estado, tipo, fechas y observaciones.</t>
-  </si>
-  <si>
-    <t>Debe poder ordenarse por fecha.</t>
-  </si>
-  <si>
     <r>
       <t>Requisito relacionado:</t>
     </r>
@@ -664,49 +509,310 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Requisito relacionado:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> RF011 - El sistema debe permitir a los empleados registrar una solicitud de vacaciones.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Requisito relacionado:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> RF012 - El sistema debe permitir a los supervisores aprobar o rechazar solicitudes de vacaciones.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Requisito relacionado:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> RF013 - El sistema debe permitir al empleado visualizar su historial de vacaciones.</t>
-    </r>
+    <t>El sistema debe permitir al administrador registrar una solicitud de permiso para un empleado.</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al administrador aprobar o rechazar solicitudes de permiso enviadas por empleados.</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al administrador consultar el historial de solicitudes de permiso por empleado.</t>
+  </si>
+  <si>
+    <t>El sistema debe mostrar al administrador un calendario general de permisos tomados y pendientes por empleados.</t>
+  </si>
+  <si>
+    <r>
+      <t>Como</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> administrador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Quiero</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> registrar una solicitud de permiso para un empleado específico</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Para</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> apoyar en la gestión de permisos cuando el empleado no pueda acceder al sistema</t>
+    </r>
+  </si>
+  <si>
+    <t>El sistema debe permitir seleccionar el nombre del empleado.</t>
+  </si>
+  <si>
+    <t>Se debe poder especificar el tipo de permiso (vacaciones, enfermedad, etc.).</t>
+  </si>
+  <si>
+    <t>Se debe ingresar una fecha de inicio y fin, y un motivo.</t>
+  </si>
+  <si>
+    <t>Definition of Ready (DoR):</t>
+  </si>
+  <si>
+    <t>El módulo de permisos está accesible.</t>
+  </si>
+  <si>
+    <t>Se cuenta con el listado de empleados cargado.</t>
+  </si>
+  <si>
+    <t>Se definieron los tipos de permiso disponibles.</t>
+  </si>
+  <si>
+    <t>Definition of Done (DoD):</t>
+  </si>
+  <si>
+    <t>La solicitud queda registrada y visible en el historial del empleado.</t>
+  </si>
+  <si>
+    <t>Se muestra un mensaje de confirmación exitoso.</t>
+  </si>
+  <si>
+    <t>El estado inicial de la solicitud es "pendiente".</t>
+  </si>
+  <si>
+    <r>
+      <t>Estimación:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3 puntos</t>
+    </r>
+  </si>
+  <si>
+    <t>HU003 - Registrar nuevo empleado</t>
+  </si>
+  <si>
+    <t>HU004 - Editar información de empleado</t>
+  </si>
+  <si>
+    <t>HU001 - Inicio de sesión</t>
+  </si>
+  <si>
+    <t>HU002 -  Cerrar sesión</t>
+  </si>
+  <si>
+    <t>HU005 - Buscar empleados</t>
+  </si>
+  <si>
+    <t>HU006 - Registrar solicitud de permiso para un empleado</t>
+  </si>
+  <si>
+    <r>
+      <t>Quiero</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> revisar y aprobar o rechazar solicitudes de permisos enviadas</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Para</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> asegurar un control adecuado sobre las ausencias laborales</t>
+    </r>
+  </si>
+  <si>
+    <t>Se puede ver la lista de solicitudes pendientes.</t>
+  </si>
+  <si>
+    <t>Se puede ver el detalle (fechas, tipo, motivo).</t>
+  </si>
+  <si>
+    <t>Se debe contar con botones para "Aprobar" o "Rechazar".</t>
+  </si>
+  <si>
+    <t>Al tomar una acción, debe registrarse con usuario, fecha y comentario.</t>
+  </si>
+  <si>
+    <t>DoR:</t>
+  </si>
+  <si>
+    <t>Hay al menos una solicitud en estado pendiente.</t>
+  </si>
+  <si>
+    <t>El usuario tiene permisos de administración.</t>
+  </si>
+  <si>
+    <t>DoD:</t>
+  </si>
+  <si>
+    <t>El estado de la solicitud cambia correctamente.</t>
+  </si>
+  <si>
+    <t>El historial registra la acción.</t>
+  </si>
+  <si>
+    <t>El empleado queda notificado (o se simula en el entorno DEMO).</t>
+  </si>
+  <si>
+    <r>
+      <t>Estimación:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 5 puntos</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Quiero</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> consultar todas las solicitudes de permiso de un empleado</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Para</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hacer seguimiento de ausencias por tipo, fecha y estado</t>
+    </r>
+  </si>
+  <si>
+    <t>Debe poder buscar al empleado por nombre o ID.</t>
+  </si>
+  <si>
+    <t>Debe incluir estado (pendiente, aprobado, rechazado) y fechas.</t>
+  </si>
+  <si>
+    <t>Se cuenta con solicitudes registradas en el sistema.</t>
+  </si>
+  <si>
+    <t>El historial muestra datos exactos y completos.</t>
+  </si>
+  <si>
+    <t>Permite exportar o visualizar en un formato ordenado (si aplica).</t>
+  </si>
+  <si>
+    <r>
+      <t>Quiero</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ver un calendario de permisos tomados y pendientes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Para</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tener una vista general del personal ausente y planificar recursos</t>
+    </r>
+  </si>
+  <si>
+    <t>El calendario debe mostrar marcadas las fechas por empleado.</t>
+  </si>
+  <si>
+    <t>Debe poderse filtrar por tipo de permiso o área.</t>
+  </si>
+  <si>
+    <t>Permite ver los detalles al hacer clic en una fecha o evento.</t>
+  </si>
+  <si>
+    <t>Hay permisos registrados.</t>
+  </si>
+  <si>
+    <t>El módulo calendario está accesible.</t>
+  </si>
+  <si>
+    <t>El calendario carga correctamente los datos.</t>
+  </si>
+  <si>
+    <t>El diseño es claro y navegable.</t>
+  </si>
+  <si>
+    <t>HU007 - Aprobar o rechazar solicitud de permiso</t>
+  </si>
+  <si>
+    <t>HU008 - Visualizar historial de permisos de un empleado</t>
+  </si>
+  <si>
+    <t>HU009 - Visualizar calendario general de permisos</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1200,7 @@
   <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1249,7 +1355,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
@@ -1257,7 +1363,7 @@
         <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
@@ -1265,7 +1371,7 @@
         <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
@@ -1273,43 +1379,43 @@
         <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -1317,31 +1423,31 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -1350,39 +1456,39 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
         <v>48</v>
-      </c>
-      <c r="C36" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" t="s">
         <v>49</v>
-      </c>
-      <c r="C37" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
         <v>50</v>
-      </c>
-      <c r="C38" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
         <v>51</v>
-      </c>
-      <c r="C39" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -1391,31 +1497,31 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -1424,32 +1530,32 @@
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C51" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1462,8 +1568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499CA4CF-450D-45CD-81A2-DB060D33A0E2}">
   <dimension ref="A1:Z110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1503,7 +1609,7 @@
     </row>
     <row r="3" spans="1:26" ht="18" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -1511,7 +1617,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
@@ -1519,22 +1625,22 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
@@ -1542,22 +1648,22 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="18" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1565,7 +1671,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
@@ -1573,22 +1679,22 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
@@ -1596,22 +1702,22 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="18" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -1620,7 +1726,7 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
@@ -1628,22 +1734,22 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="9" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="9" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
@@ -1651,22 +1757,22 @@
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" s="8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="18" x14ac:dyDescent="0.3">
       <c r="B44" s="10" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -1676,7 +1782,7 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
@@ -1684,22 +1790,22 @@
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="9" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="9" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
@@ -1707,22 +1813,22 @@
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="8" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" s="8" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="18" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
@@ -1731,7 +1837,7 @@
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.3">
@@ -1739,193 +1845,427 @@
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="9" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="8"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="8"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="8"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="9"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="9"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="8"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="8"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="8"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="8"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B108" s="8"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B109" s="8"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F444C67F-764A-4B8E-BDED-33977D896FBD}">
+  <dimension ref="B1:G89"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="2:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="B71" s="10" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B28" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="B52" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B54" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B56" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B58" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61" s="8"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B62" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B63" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B65" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B66" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B67" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B70" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B72" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B74" s="8"/>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B75" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B76" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B77" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B79" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B80" s="8"/>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B81" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B74" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B77" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B78" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B79" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="B85" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C85" s="6"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B87" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B88" s="8"/>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B89" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B90" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B91" s="9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B93" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B94" s="8"/>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B95" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B96" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B97" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="B99" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-      <c r="E99" s="6"/>
-      <c r="F99" s="6"/>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B101" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B102" s="8"/>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B103" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B104" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B105" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B107" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B108" s="8"/>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B109" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B110" s="8" t="s">
-        <v>123</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B89" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se diseño y ejecuto nuevos casos de prueba para las HU del modulo Leave
</commit_message>
<xml_diff>
--- a/01-Requisitos-Historias_Usuario/Requisitos-Historias_Usuario.xlsx
+++ b/01-Requisitos-Historias_Usuario/Requisitos-Historias_Usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DIEGO\Desktop\Practicas-Personales\QA\Portafolio QA Automatizacion\01-Requisitos-Historias_Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456FD1ED-8D6D-46EB-BD1B-DAF7003F4161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27843A6-519B-4B20-B22F-5B2C0954DBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="157">
   <si>
     <t>Requisitos Funcionales – OrangeHRM Demo</t>
   </si>
@@ -518,9 +518,6 @@
     <t>El sistema debe permitir al administrador consultar el historial de solicitudes de permiso por empleado.</t>
   </si>
   <si>
-    <t>El sistema debe mostrar al administrador un calendario general de permisos tomados y pendientes por empleados.</t>
-  </si>
-  <si>
     <r>
       <t>Como</t>
     </r>
@@ -569,12 +566,6 @@
     <t>El sistema debe permitir seleccionar el nombre del empleado.</t>
   </si>
   <si>
-    <t>Se debe poder especificar el tipo de permiso (vacaciones, enfermedad, etc.).</t>
-  </si>
-  <si>
-    <t>Se debe ingresar una fecha de inicio y fin, y un motivo.</t>
-  </si>
-  <si>
     <t>Definition of Ready (DoR):</t>
   </si>
   <si>
@@ -590,15 +581,9 @@
     <t>Definition of Done (DoD):</t>
   </si>
   <si>
-    <t>La solicitud queda registrada y visible en el historial del empleado.</t>
-  </si>
-  <si>
     <t>Se muestra un mensaje de confirmación exitoso.</t>
   </si>
   <si>
-    <t>El estado inicial de la solicitud es "pendiente".</t>
-  </si>
-  <si>
     <r>
       <t>Estimación:</t>
     </r>
@@ -740,9 +725,6 @@
     </r>
   </si>
   <si>
-    <t>Debe poder buscar al empleado por nombre o ID.</t>
-  </si>
-  <si>
     <t>Debe incluir estado (pendiente, aprobado, rechazado) y fechas.</t>
   </si>
   <si>
@@ -756,6 +738,71 @@
   </si>
   <si>
     <r>
+      <t>Para</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tener una vista general del personal ausente y planificar recursos</t>
+    </r>
+  </si>
+  <si>
+    <t>Debe poderse filtrar por tipo de permiso o área.</t>
+  </si>
+  <si>
+    <t>Hay permisos registrados.</t>
+  </si>
+  <si>
+    <t>El diseño es claro y navegable.</t>
+  </si>
+  <si>
+    <t>HU007 - Aprobar o rechazar solicitud de permiso</t>
+  </si>
+  <si>
+    <t>HU008 - Visualizar historial de permisos de un empleado</t>
+  </si>
+  <si>
+    <r>
+      <t>Se debe poder especificar el tipo de permiso (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vacaciones</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, enfermedad, etc.).</t>
+    </r>
+  </si>
+  <si>
+    <t>El estado inicial de la solicitud es "schedule (agendado)".</t>
+  </si>
+  <si>
+    <t>Se debe ingresar una fecha de inicio y fin (despues de la fecha actual), y un motivo.</t>
+  </si>
+  <si>
+    <t>HU009 - Visualizar lista general de permisos por fecha</t>
+  </si>
+  <si>
+    <r>
       <t>Quiero</t>
     </r>
     <r>
@@ -766,53 +813,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> ver un calendario de permisos tomados y pendientes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Para</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> tener una vista general del personal ausente y planificar recursos</t>
-    </r>
-  </si>
-  <si>
-    <t>El calendario debe mostrar marcadas las fechas por empleado.</t>
-  </si>
-  <si>
-    <t>Debe poderse filtrar por tipo de permiso o área.</t>
-  </si>
-  <si>
-    <t>Permite ver los detalles al hacer clic en una fecha o evento.</t>
-  </si>
-  <si>
-    <t>Hay permisos registrados.</t>
-  </si>
-  <si>
-    <t>El módulo calendario está accesible.</t>
-  </si>
-  <si>
-    <t>El calendario carga correctamente los datos.</t>
-  </si>
-  <si>
-    <t>El diseño es claro y navegable.</t>
-  </si>
-  <si>
-    <t>HU007 - Aprobar o rechazar solicitud de permiso</t>
-  </si>
-  <si>
-    <t>HU008 - Visualizar historial de permisos de un empleado</t>
-  </si>
-  <si>
-    <t>HU009 - Visualizar calendario general de permisos</t>
+      <t xml:space="preserve"> ver una lista de permisos tomados y pendientes por fecha</t>
+    </r>
+  </si>
+  <si>
+    <t>El módulo leave está accesible.</t>
+  </si>
+  <si>
+    <t>Se carga correctamente los datos.</t>
+  </si>
+  <si>
+    <t>Debe poder buscar al empleado por nombre.</t>
+  </si>
+  <si>
+    <t>La lista debe mostrar los permisos dentro del intervalo de fechas.</t>
+  </si>
+  <si>
+    <t>Permite ver los detalles del permiso (fecha, nombre, tipo, estado, comentario, etc)</t>
+  </si>
+  <si>
+    <t>El sistema debe mostrar al administrador un listado general de permisos tomados y pendientes por empleados.</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1220,7 @@
   <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1379,7 +1399,7 @@
         <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
@@ -1609,7 +1629,7 @@
     </row>
     <row r="3" spans="1:26" ht="18" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -1663,7 +1683,7 @@
     </row>
     <row r="16" spans="1:26" ht="18" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1717,7 +1737,7 @@
     </row>
     <row r="30" spans="2:6" ht="18" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -1772,7 +1792,7 @@
     </row>
     <row r="44" spans="2:7" ht="18" x14ac:dyDescent="0.3">
       <c r="B44" s="10" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -1828,7 +1848,7 @@
     </row>
     <row r="58" spans="2:6" ht="18" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
@@ -1922,10 +1942,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F444C67F-764A-4B8E-BDED-33977D896FBD}">
-  <dimension ref="B1:G89"/>
+  <dimension ref="B1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1935,7 +1955,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="18" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -1945,17 +1965,17 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -1968,22 +1988,22 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
-        <v>109</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
@@ -1991,22 +2011,22 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -2014,228 +2034,228 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="B28" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B27" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" s="1" t="s">
-        <v>71</v>
+      <c r="B34" s="8" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" s="8" t="s">
-        <v>130</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B40" s="1" t="s">
-        <v>131</v>
+      <c r="B40" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B42" s="8" t="s">
-        <v>133</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B44" s="1" t="s">
-        <v>134</v>
+      <c r="B44" s="8" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B47" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="B52" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="B51" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B58" s="1" t="s">
-        <v>71</v>
+      <c r="B58" s="8" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59" s="8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="8" t="s">
-        <v>142</v>
-      </c>
+      <c r="B60" s="8"/>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="8"/>
+      <c r="B61" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B62" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B63" s="8" t="s">
-        <v>143</v>
+      <c r="B62" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B64" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B65" s="1" t="s">
-        <v>134</v>
+      <c r="B65" s="8" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B67" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="B70" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B69" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B71" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B74" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B75" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B76" s="1" t="s">
-        <v>71</v>
+      <c r="B76" s="8" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="8" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B79" s="8" t="s">
-        <v>150</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B80" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B81" s="1" t="s">
-        <v>131</v>
+      <c r="B81" s="8" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.3">
@@ -2243,29 +2263,24 @@
         <v>151</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B83" s="8" t="s">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="8" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B85" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B87" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B89" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregan nuevos casos de prueba a HU-006 y se ejecutan los de HU-006, HU-008, HU-009
</commit_message>
<xml_diff>
--- a/01-Requisitos-Historias_Usuario/Requisitos-Historias_Usuario.xlsx
+++ b/01-Requisitos-Historias_Usuario/Requisitos-Historias_Usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DIEGO\Desktop\Practicas-Personales\QA\Portafolio QA Automatizacion\01-Requisitos-Historias_Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27843A6-519B-4B20-B22F-5B2C0954DBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DA6D5E-0843-4A3D-B72A-31F85C3C74DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1944,8 +1944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F444C67F-764A-4B8E-BDED-33977D896FBD}">
   <dimension ref="B1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Se agregan y ejecutan nuevos casos de prueba a HU-008 y HU-009, ademas se completan los CP en redaccion gherkin
</commit_message>
<xml_diff>
--- a/01-Requisitos-Historias_Usuario/Requisitos-Historias_Usuario.xlsx
+++ b/01-Requisitos-Historias_Usuario/Requisitos-Historias_Usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DIEGO\Desktop\Practicas-Personales\QA\Portafolio QA Automatizacion\01-Requisitos-Historias_Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DA6D5E-0843-4A3D-B72A-31F85C3C74DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F615051-E05A-4074-B793-448E62B9B9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -799,9 +799,6 @@
     <t>Se debe ingresar una fecha de inicio y fin (despues de la fecha actual), y un motivo.</t>
   </si>
   <si>
-    <t>HU009 - Visualizar lista general de permisos por fecha</t>
-  </si>
-  <si>
     <r>
       <t>Quiero</t>
     </r>
@@ -833,6 +830,9 @@
   </si>
   <si>
     <t>El sistema debe mostrar al administrador un listado general de permisos tomados y pendientes por empleados.</t>
+  </si>
+  <si>
+    <t>HU009 - Visualizar lista general de permisos de los empleados por fecha</t>
   </si>
 </sst>
 </file>
@@ -1399,7 +1399,7 @@
         <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
@@ -1942,10 +1942,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F444C67F-764A-4B8E-BDED-33977D896FBD}">
-  <dimension ref="B1:G88"/>
+  <dimension ref="B1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
@@ -2194,61 +2194,63 @@
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B65" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B66" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B69" s="10" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B71" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B75" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B76" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B77" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B78" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
         <v>126</v>
       </c>
@@ -2260,7 +2262,7 @@
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.3">
@@ -2270,7 +2272,7 @@
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>